<commit_message>
Cambia numero de la segundo isosceles
</commit_message>
<xml_diff>
--- a/Caminos McCabe.xlsx
+++ b/Caminos McCabe.xlsx
@@ -156,6 +156,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -165,7 +166,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +449,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="A1:O12"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,26 +459,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -488,10 +488,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -505,7 +505,7 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -518,10 +518,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -534,7 +534,7 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -550,10 +550,10 @@
         <v>4</v>
       </c>
       <c r="F4" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -565,7 +565,7 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -587,10 +587,10 @@
         <v>6</v>
       </c>
       <c r="H5" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -600,7 +600,7 @@
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -625,10 +625,10 @@
         <v>7</v>
       </c>
       <c r="I6" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -637,7 +637,7 @@
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -665,10 +665,10 @@
         <v>8</v>
       </c>
       <c r="J7" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K7" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -676,7 +676,7 @@
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -716,12 +716,12 @@
         <v>12</v>
       </c>
       <c r="N8" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -761,12 +761,12 @@
         <v>13</v>
       </c>
       <c r="N9" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -803,15 +803,15 @@
         <v>14</v>
       </c>
       <c r="M10" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N10" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
@@ -851,14 +851,14 @@
         <v>15</v>
       </c>
       <c r="N11" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O11" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -898,10 +898,10 @@
         <v>15</v>
       </c>
       <c r="N12" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O12" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>